<commit_message>
Add materials in Report displaying
</commit_message>
<xml_diff>
--- a/JOI Summary.xlsx
+++ b/JOI Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>JOI Summary 2021</t>
   </si>
@@ -50,15 +50,33 @@
     <t>Scope of Work</t>
   </si>
   <si>
+    <t>Materials Offer</t>
+  </si>
+  <si>
+    <t>Materials QTY</t>
+  </si>
+  <si>
+    <t>Materials UOM</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Status Remarks</t>
+  </si>
+  <si>
     <t>Supplier</t>
   </si>
   <si>
     <t>Payment Terms</t>
   </si>
   <si>
+    <t>Materials Unit Price</t>
+  </si>
+  <si>
+    <t>Materials Total Price</t>
+  </si>
+  <si>
     <t>Unit Price</t>
   </si>
   <si>
@@ -71,93 +89,42 @@
     <t>JOR 2021-1-CNPR</t>
   </si>
   <si>
-    <t>sample purpose</t>
-  </si>
-  <si>
-    <t>2021-05-05</t>
+    <t>SAMPLE PURPOSE BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>2021-08-24</t>
   </si>
   <si>
     <t>PJOR 2021-1-1000-CNPR</t>
   </si>
   <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>item testing 1</t>
-  </si>
-  <si>
-    <t>JO Issued</t>
-  </si>
-  <si>
-    <t>2GO Express, Inc.</t>
-  </si>
-  <si>
-    <t>Freight Collect / Prepaid</t>
-  </si>
-  <si>
-    <t>PHP 150.00</t>
-  </si>
-  <si>
-    <t>P-1002-CNPR</t>
+    <t>SAMPLE REQUEST BY HR ADMIN</t>
+  </si>
+  <si>
+    <t>lot/s</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>trials</t>
+  </si>
+  <si>
+    <t>Fully Delivered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.24.2021 - Delivered DR# 1000-CNPR (1.00 lot/s)
+08.24.2021 - Delivered DR# 1001-CNPR (0.00 lot/s)
+</t>
   </si>
   <si>
     <t xml:space="preserve"> Tough Performance AutoWorkz</t>
   </si>
   <si>
-    <t xml:space="preserve"> 150.00</t>
-  </si>
-  <si>
-    <t>P-1003-CNPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1500.00</t>
-  </si>
-  <si>
-    <t>P-1004-CNPR</t>
-  </si>
-  <si>
-    <t>A-one Industrial Sales</t>
-  </si>
-  <si>
-    <t>CENJO-EM007-100-CNPR</t>
-  </si>
-  <si>
-    <t>Retrofitting of UG40 Hydraulic</t>
-  </si>
-  <si>
-    <t>2021-05-06</t>
-  </si>
-  <si>
-    <t>PCENJO-EM007-100-1005-CNPR</t>
-  </si>
-  <si>
-    <t>sdfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05.13.2021 - Delivered DR# 1010-CNPR
-</t>
-  </si>
-  <si>
-    <t>PHP 324.00</t>
-  </si>
-  <si>
-    <t>PCENJO-EM007-100-1006-CNPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05.13.2021 - Delivered DR# 1011-CNPR
-</t>
-  </si>
-  <si>
-    <t>PCENJO-EM007-100-1007-CNPR</t>
-  </si>
-  <si>
-    <t>Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum</t>
-  </si>
-  <si>
-    <t>A.C. Parts Merchandising</t>
-  </si>
-  <si>
-    <t>PHP 3453.00</t>
+    <t>AUD 20.0000</t>
+  </si>
+  <si>
+    <t>PHP 50.00</t>
   </si>
 </sst>
 </file>
@@ -194,7 +161,7 @@
       <name val="Arial Black"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,13 +173,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffecd0"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFb9ffb9"/>
+        <fgColor rgb="FFbcffc7"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -237,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -260,18 +221,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -573,32 +522,38 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="27.13623" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="36.419678" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="129.682617" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="43.560791" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="34.134521" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="58.842773" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="34.134521" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="9.283447" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -607,12 +562,12 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:21">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -658,293 +613,85 @@
       <c r="O4" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="P4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:21">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F5" s="6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6">
-        <v>3</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="6">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="6">
-        <v>450</v>
-      </c>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="N5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6">
-        <v>7</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="6">
-        <v>10500</v>
-      </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="8" t="s">
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="R5" s="6">
+        <v>40</v>
+      </c>
+      <c r="S5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10">
-        <v>5</v>
-      </c>
-      <c r="G9" s="10">
-        <v>5</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="10">
-        <v>1620</v>
-      </c>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10">
-        <v>5</v>
-      </c>
-      <c r="G10" s="10">
-        <v>5</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="10">
-        <v>1620</v>
-      </c>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N11" s="6">
-        <v>10359</v>
-      </c>
-      <c r="O11" s="5"/>
+      <c r="T5" s="6">
+        <v>50</v>
+      </c>
+      <c r="U5" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Create function for update status in Reports and add calculation for rfd
</commit_message>
<xml_diff>
--- a/JOI Summary.xlsx
+++ b/JOI Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>JOI Summary 2021</t>
   </si>
@@ -89,42 +89,62 @@
     <t>JOR 2021-1-CNPR</t>
   </si>
   <si>
-    <t>SAMPLE PURPOSE BY HR ADMIN</t>
-  </si>
-  <si>
-    <t>2021-08-24</t>
+    <t>Repair of entrance front door glass.</t>
+  </si>
+  <si>
+    <t>2021-09-03</t>
   </si>
   <si>
     <t>PJOR 2021-1-1000-CNPR</t>
   </si>
   <si>
-    <t>SAMPLE REQUEST BY HR ADMIN</t>
-  </si>
-  <si>
-    <t>lot/s</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>trials</t>
-  </si>
-  <si>
-    <t>Fully Delivered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08.24.2021 - Delivered DR# 1000-CNPR (1.00 lot/s)
-08.24.2021 - Delivered DR# 1001-CNPR (0.00 lot/s)
-</t>
+    <t>Syndey Sinoro</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Aragay Nars</t>
+  </si>
+  <si>
+    <t>Testing Offer</t>
+  </si>
+  <si>
+    <t>Partially Delivered</t>
+  </si>
+  <si>
+    <t>Testing jashdk jka sdjk
+klsajdl k</t>
   </si>
   <si>
     <t xml:space="preserve"> Tough Performance AutoWorkz</t>
   </si>
   <si>
-    <t>AUD 20.0000</t>
-  </si>
-  <si>
-    <t>PHP 50.00</t>
+    <t>PHP 200.0000</t>
+  </si>
+  <si>
+    <t>PHP 100.00</t>
+  </si>
+  <si>
+    <t>2021-09-06</t>
+  </si>
+  <si>
+    <t>PJOR 2021-1-1004-CNPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Item no. 4 sample</t>
+  </si>
+  <si>
+    <t>aragay nars</t>
+  </si>
+  <si>
+    <t>JO Issued</t>
+  </si>
+  <si>
+    <t>PHP 40.0000</t>
+  </si>
+  <si>
+    <t>PHP 20.00</t>
   </si>
 </sst>
 </file>
@@ -161,7 +181,7 @@
       <name val="Arial Black"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,7 +193,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFbcffc7"/>
+        <fgColor rgb="FFf7ffb9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFffecd0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -198,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -221,6 +247,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -522,28 +560,28 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="27.13623" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="43.560791" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="25.85083" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="58.842773" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="28.135986" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="34.134521" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="24.708252" bestFit="true" customWidth="true" style="0"/>
@@ -649,10 +687,10 @@
         <v>27</v>
       </c>
       <c r="F5" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>28</v>
@@ -664,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="K5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>28</v>
@@ -683,15 +721,74 @@
         <v>34</v>
       </c>
       <c r="R5" s="6">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="T5" s="6">
-        <v>50</v>
+        <v>600</v>
       </c>
       <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="10">
+        <v>40</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="10">
+        <v>20</v>
+      </c>
+      <c r="U6" s="9"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>